<commit_message>
Test Script Changes Feb 20
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DMICodeChallenge16022022\DMICodeChallenge\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB7871B-F745-49C5-B58D-15E1E6A47D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C754DD6D-ACA0-4585-B2C1-82782BB95043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>NameOfToDos</t>
   </si>
@@ -68,35 +69,35 @@
     <t>New ToDo Entry 4</t>
   </si>
   <si>
-    <t>ToDo5</t>
-  </si>
-  <si>
-    <t>New ToDo Entry 5</t>
-  </si>
-  <si>
-    <t>ToDo6</t>
-  </si>
-  <si>
-    <t>New ToDo Entry 6</t>
-  </si>
-  <si>
-    <t>ToDo7</t>
-  </si>
-  <si>
-    <t>New ToDo Entry 7</t>
-  </si>
-  <si>
-    <t>ToDo8</t>
-  </si>
-  <si>
-    <t>New ToDo Entry 8</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>baseURL</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>https://www.todobackend.com/client/index.html?https://mysterious-thicket-31854.herokuapp.com/#/completed</t>
+  </si>
+  <si>
+    <t>https://www.todobackend.com/client/index.html?https://mysterious-thicket-31854.herokuapp.com/#/active</t>
+  </si>
+  <si>
+    <t>https://www.todobackend.com/client/index.html?https://mysterious-thicket-31854.herokuapp.com/#/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +111,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -119,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -127,14 +136,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -413,11 +441,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -464,14 +490,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -480,10 +498,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236A2D5A-6DC0-4D43-8A52-341C74D738D5}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,40 +530,64 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A58F84-E9E0-4059-87B4-82DCBA6A9DA1}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="65" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="/completed" xr:uid="{4B033563-1BC0-48FD-819C-C8C07F9906B6}"/>
+    <hyperlink ref="B3" r:id="rId2" location="/active" xr:uid="{6C464FC7-65C2-4BE3-AB3D-75351A36E028}"/>
+    <hyperlink ref="B4" r:id="rId3" location="/" xr:uid="{1BA0B0DF-DE9E-48D2-A0B0-B31630C03FAD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>